<commit_message>
add evaluation param cluster and threshold
</commit_message>
<xml_diff>
--- a/server/main_algorithm/resources/surahCek.xlsx
+++ b/server/main_algorithm/resources/surahCek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA UB\Refrensi project\react-python-skripsi\server\main_algorithm\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1357338-AB21-4235-A7C5-8DDE4CCD3016}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496ECE67-519A-42B8-98D5-4E0D783D7DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,21 +52,6 @@
     <t>(yaitu) Jalan orang-orang yang telah Engkau beri nikmat kepada mereka; bukan (jalan) mereka yang dimurkai dan bukan (pula jalan) mereka yang sesat.</t>
   </si>
   <si>
-    <t>Apakah kamu tidak memperhatikan bagaimana Tuhanmu telah bertindak terhadap tentara bergajah?</t>
-  </si>
-  <si>
-    <t>Bukankah Dia telah menjadikan tipu daya mereka (untuk menghancurkan Ka´bah) itu sia-sia?</t>
-  </si>
-  <si>
-    <t>dan Dia mengirimkan kapada mereka burung yang berbondong-bondong,</t>
-  </si>
-  <si>
-    <t>yang melempari mereka dengan batu (berasal) dari tanah yang terbakar,</t>
-  </si>
-  <si>
-    <t>lalu Dia menjadikan mereka seperti daun-daun yang dimakan (ulat).</t>
-  </si>
-  <si>
     <t>Tahukah kamu (orang) yang mendustakan agama?</t>
   </si>
   <si>
@@ -143,6 +128,21 @@
   </si>
   <si>
     <t>Dan terhadap nikmat Tuhanmu, maka hendaklah kamu siarkan.</t>
+  </si>
+  <si>
+    <t>Binasalah kedua tangan Abu Lahab dan sesungguhnya dia akan binasa.</t>
+  </si>
+  <si>
+    <t>Tidaklah berfaedah kepadanya harta bendanya dan apa yang ia usahakan.</t>
+  </si>
+  <si>
+    <t>Kelak dia akan masuk ke dalam api yang bergejolak.</t>
+  </si>
+  <si>
+    <t>Dan (begitu pula) istrinya, pembawa kayu bakar.</t>
+  </si>
+  <si>
+    <t>Yang di lehernya ada tali dari sabut.</t>
   </si>
 </sst>
 </file>
@@ -1039,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1138,59 +1138,59 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B11" s="2">
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B12" s="2">
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B13" s="2">
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -1201,7 +1201,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1212,7 +1212,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -1223,7 +1223,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -1234,7 +1234,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -1245,7 +1245,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1256,7 +1256,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -1267,7 +1267,7 @@
         <v>7</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1278,7 +1278,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1289,7 +1289,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1300,7 +1300,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
@@ -1311,7 +1311,7 @@
         <v>4</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -1322,7 +1322,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
@@ -1333,7 +1333,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
@@ -1344,7 +1344,7 @@
         <v>7</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1355,7 +1355,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1366,7 +1366,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -1377,7 +1377,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -1388,7 +1388,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
@@ -1399,7 +1399,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
@@ -1410,7 +1410,7 @@
         <v>5</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -1421,7 +1421,7 @@
         <v>6</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
@@ -1432,7 +1432,7 @@
         <v>7</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
@@ -1443,7 +1443,7 @@
         <v>8</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -1454,7 +1454,7 @@
         <v>9</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -1465,7 +1465,7 @@
         <v>10</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -1476,7 +1476,7 @@
         <v>11</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>